<commit_message>
Rebuild index after corruption
</commit_message>
<xml_diff>
--- a/eth_purchases.xlsx
+++ b/eth_purchases.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,6 +872,176 @@
         <v>12.18304729394199</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>46006</v>
+      </c>
+      <c r="B26" t="n">
+        <v>102259</v>
+      </c>
+      <c r="C26" t="n">
+        <v>318536785</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2964.18310546875</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10.47025078220676</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>46013</v>
+      </c>
+      <c r="B27" t="n">
+        <v>98852</v>
+      </c>
+      <c r="C27" t="n">
+        <v>294578960</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3006.07373046875</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10.29435269453544</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B28" t="n">
+        <v>44463</v>
+      </c>
+      <c r="C28" t="n">
+        <v>131610480</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2934.538330078125</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6.904078079755683</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B29" t="n">
+        <v>32977</v>
+      </c>
+      <c r="C29" t="n">
+        <v>100579850</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3226.13037109375</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.945821750849223</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B30" t="n">
+        <v>24266</v>
+      </c>
+      <c r="C30" t="n">
+        <v>76923220</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3092.3251953125</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5.100413773821187</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>46041</v>
+      </c>
+      <c r="B31" t="n">
+        <v>35268</v>
+      </c>
+      <c r="C31" t="n">
+        <v>116540860</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3186.62109375</v>
+      </c>
+      <c r="E31" t="n">
+        <v>6.148890077690821</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>46048</v>
+      </c>
+      <c r="B32" t="n">
+        <v>40302</v>
+      </c>
+      <c r="C32" t="n">
+        <v>120099960</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2926.45703125</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.573090512286873</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>46055</v>
+      </c>
+      <c r="B33" t="n">
+        <v>41788</v>
+      </c>
+      <c r="C33" t="n">
+        <v>141404692</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2344.356689453125</v>
+      </c>
+      <c r="E33" t="n">
+        <v>6.69317386039803</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="B34" t="n">
+        <v>40613</v>
+      </c>
+      <c r="C34" t="n">
+        <v>88536340</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2103.567626953125</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6.598403184030338</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>46070</v>
+      </c>
+      <c r="B35" t="n">
+        <v>45759</v>
+      </c>
+      <c r="C35" t="n">
+        <v>91289205</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1992.1943359375</v>
+      </c>
+      <c r="E35" t="n">
+        <v>7.003974814820833</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>